<commit_message>
Estoy acabando con los reportes, graficos listos, excel listo, dar chequeada
</commit_message>
<xml_diff>
--- a/fabricas.xlsx
+++ b/fabricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +501,52 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Fabrica 3:</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EE.UU.</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Fabrica 4:</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bandai Namco</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Acabamos reportes, pero lo vamos a cambiar en los numericos, horizontal/ nombres_fabricas, vertical/valores numericos
</commit_message>
<xml_diff>
--- a/fabricas.xlsx
+++ b/fabricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,19 +509,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lego</t>
+          <t>Hashlin Comelona</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>EE.UU.</t>
+          <t>India</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -532,19 +532,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bandai Namco</t>
+          <t>Serquen</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Cerru</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Fabrica 5:</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Remedial</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cerru</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E6" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregue un nuevo metodo en fabrica para asignar las unidades a los juguetes y actualice el agregar fabrica
</commit_message>
<xml_diff>
--- a/fabricas.xlsx
+++ b/fabricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,65 +509,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hashlin Comelona</t>
+          <t>adfs</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Brasil</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Fabrica 4:</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Serquen</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Cerru</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Fabrica 5:</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Remedial</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cerru</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1300</v>
-      </c>
-      <c r="E6" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminado, periodo de pruebas
</commit_message>
<xml_diff>
--- a/fabricas.xlsx
+++ b/fabricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,19 +509,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>adfs</t>
+          <t>Lego</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Brasil</t>
+          <t>EE.UU.</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>10000</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Fabrica 4:</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bandai Namco</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregue un nuevo poryecto
</commit_message>
<xml_diff>
--- a/fabricas.xlsx
+++ b/fabricas.xlsx
@@ -509,19 +509,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lego</t>
+          <t>Cualquiera</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>1241</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>15000</v>
+        <v>16000</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
listo el excel con el inventario
</commit_message>
<xml_diff>
--- a/fabricas.xlsx
+++ b/fabricas.xlsx
@@ -509,19 +509,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cualquiera</t>
+          <t>LEGO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>1241</t>
+          <t>Cerru</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>16000</v>
+        <v>12000</v>
       </c>
       <c r="E4" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>